<commit_message>
reduce PWM to 10kHz
</commit_message>
<xml_diff>
--- a/current-sense-jig/Plots.xlsx
+++ b/current-sense-jig/Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/330982bbf88a3d54/Desktop/ENPH 459 - AI Air Hockey/current-sense-jig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{3242610A-DAB0-44C0-BEBC-9EF3C6DED397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{751B8CC5-09C4-489E-83E6-37EDEEA48562}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{3242610A-DAB0-44C0-BEBC-9EF3C6DED397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07489234-7E91-4B88-ADD2-41D0070F1DD5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C213672D-D1B3-410F-BE59-45F4EFB387BF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Duty cycle</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>sample rate is WAY too slow</t>
   </si>
 </sst>
 </file>
@@ -13758,6 +13761,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16336,7 +16343,7 @@
   <dimension ref="A1:AK397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16701,6 +16708,9 @@
       <c r="A22">
         <v>1.92</v>
       </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
       <c r="J22">
         <v>3.3</v>
       </c>

</xml_diff>